<commit_message>
check test for update cache from file with disc
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>8dac7529-5bcb-4f7b-b345-6ddf5eef1d3f</t>
   </si>
@@ -178,31 +178,7 @@
     <t>Это купаж высококачественных солодовых и зерновых виски, выдержанных как минимум в течение 12 лет</t>
   </si>
   <si>
-    <t>cea94b43-242c-42bc-8d89-5a470660568c</t>
-  </si>
-  <si>
-    <t>TEST_TO_ADD</t>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>ab5fb35a-6e7c-46d0-923e-d0128f661315</t>
-  </si>
-  <si>
-    <t>ntcn</t>
-  </si>
-  <si>
-    <t>xkjhngf</t>
-  </si>
-  <si>
-    <t>c59248d4-691b-4128-a486-8c733317cda5</t>
-  </si>
-  <si>
-    <t>;IKSFD</t>
-  </si>
-  <si>
-    <t>kdjfgh</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -274,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -297,7 +273,7 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -305,6 +281,9 @@
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -626,13 +605,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="43.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="56.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="77.7192857142857" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="41.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="43.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="56.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="13" width="21.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="77.7192857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="14" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="15" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -940,10 +919,10 @@
         <v>54</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -953,13 +932,13 @@
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="4"/>
       <c r="B20" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>59</v>
+      <c r="D20" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="10"/>
@@ -969,25 +948,27 @@
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>61</v>
+      <c r="D21" s="11" t="s">
+        <v>54</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>62</v>
+      <c r="E21" s="11" t="s">
+        <v>54</v>
       </c>
-      <c r="F21" s="10">
-        <v>10.2</v>
+      <c r="F21" s="10"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+      <c r="A22" s="8" t="s">
+        <v>54</v>
       </c>
-      <c r="G21" s="4">
-        <v>5</v>
+      <c r="B22" s="8" t="s">
+        <v>54</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="C22" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="10"/>
@@ -995,9 +976,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="9"/>
+      <c r="B23" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>54</v>
+      </c>
       <c r="E23" s="9"/>
       <c r="F23" s="10"/>
       <c r="G23" s="4"/>
@@ -1005,9 +992,15 @@
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
+      <c r="C24" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>54</v>
+      </c>
       <c r="F24" s="10"/>
       <c r="G24" s="4"/>
     </row>

</xml_diff>

<commit_message>
added id from file
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>8dac7529-5bcb-4f7b-b345-6ddf5eef1d3f</t>
   </si>
@@ -177,9 +177,6 @@
   <si>
     <t>Это купаж высококачественных солодовых и зерновых виски, выдержанных как минимум в течение 12 лет</t>
   </si>
-  <si>
-    <t/>
-  </si>
 </sst>
 </file>
 
@@ -250,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -273,7 +270,7 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -281,9 +278,6 @@
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -605,13 +599,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="41.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="43.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="56.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="77.7192857142857" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="14" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="15" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="41.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="43.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="56.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="21.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="77.7192857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -911,19 +905,13 @@
         <v>520.08</v>
       </c>
       <c r="G18" s="4">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>54</v>
-      </c>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="10"/>
@@ -931,15 +919,9 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="4"/>
-      <c r="B20" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>54</v>
-      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="10"/>
       <c r="G20" s="4"/>
@@ -947,28 +929,16 @@
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>54</v>
-      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
       <c r="F21" s="10"/>
       <c r="G21" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>54</v>
-      </c>
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="10"/>
@@ -976,15 +946,9 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="4"/>
-      <c r="B23" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>54</v>
-      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="10"/>
       <c r="G23" s="4"/>
@@ -992,15 +956,9 @@
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>54</v>
-      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="10"/>
       <c r="G24" s="4"/>
     </row>

</xml_diff>